<commit_message>
update beauty, MG, PSS dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -176,6 +176,27 @@
   </si>
   <si>
     <t>CA-PQ3R9NMD</t>
+  </si>
+  <si>
+    <t>CA-ULJZ6R39</t>
+  </si>
+  <si>
+    <t>CA-BSCXQNUS</t>
+  </si>
+  <si>
+    <t>CA-A2JVHZJQ</t>
+  </si>
+  <si>
+    <t>CA-0ZQMQRYY</t>
+  </si>
+  <si>
+    <t>CA-LAZWE1BF</t>
+  </si>
+  <si>
+    <t>CA-T1K15L9H</t>
+  </si>
+  <si>
+    <t>CA-HU5809FQ</t>
   </si>
 </sst>
 </file>
@@ -600,7 +621,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
update field beauty - MDLWL
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="200">
   <si>
     <t>id</t>
   </si>
@@ -602,6 +602,30 @@
   </si>
   <si>
     <t>CA-KDZKMTO8</t>
+  </si>
+  <si>
+    <t>CA-ESP9MEVO</t>
+  </si>
+  <si>
+    <t>CA-HM7BFJK9</t>
+  </si>
+  <si>
+    <t>CA-ASTM7W1T</t>
+  </si>
+  <si>
+    <t>CA-7WC8DBSI</t>
+  </si>
+  <si>
+    <t>CA-ABOL4BN8</t>
+  </si>
+  <si>
+    <t>CA-X3DUHCV6</t>
+  </si>
+  <si>
+    <t>CA-MXF89URQ</t>
+  </si>
+  <si>
+    <t>CA-C4ENCTM5</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1050,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
update coupon code for MWL
</commit_message>
<xml_diff>
--- a/src/test/resources/Genetics.xlsx
+++ b/src/test/resources/Genetics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="233">
   <si>
     <t>id</t>
   </si>
@@ -626,6 +626,105 @@
   </si>
   <si>
     <t>CA-C4ENCTM5</t>
+  </si>
+  <si>
+    <t>CA-DGY7TBQT</t>
+  </si>
+  <si>
+    <t>CA-L67KFN92</t>
+  </si>
+  <si>
+    <t>CA-VGZYIC1F</t>
+  </si>
+  <si>
+    <t>CA-BP5SQV3N</t>
+  </si>
+  <si>
+    <t>CA-XHLFG356</t>
+  </si>
+  <si>
+    <t>CA-NM5MMCTS</t>
+  </si>
+  <si>
+    <t>CA-IR3DEROF</t>
+  </si>
+  <si>
+    <t>CA-05C4B9XO</t>
+  </si>
+  <si>
+    <t>CA-E47GDQ3S</t>
+  </si>
+  <si>
+    <t>CA-EZG1CL4Y</t>
+  </si>
+  <si>
+    <t>CA-BMPI7E4Z</t>
+  </si>
+  <si>
+    <t>CA-GNDWV523</t>
+  </si>
+  <si>
+    <t>CA-Z8IS68NQ</t>
+  </si>
+  <si>
+    <t>CA-CWJB8WCJ</t>
+  </si>
+  <si>
+    <t>CA-HPMPCA3A</t>
+  </si>
+  <si>
+    <t>CA-P4S70DL6</t>
+  </si>
+  <si>
+    <t>CA-9PSA5UUI</t>
+  </si>
+  <si>
+    <t>CA-EE7J2LBD</t>
+  </si>
+  <si>
+    <t>CA-2TUGL3MW</t>
+  </si>
+  <si>
+    <t>CA-LSLC7SO4</t>
+  </si>
+  <si>
+    <t>CA-TBEB27H3</t>
+  </si>
+  <si>
+    <t>CA-BV4DBYNK</t>
+  </si>
+  <si>
+    <t>CA-32M2VM68</t>
+  </si>
+  <si>
+    <t>CA-36SAGAW1</t>
+  </si>
+  <si>
+    <t>CA-5Q2L9UB6</t>
+  </si>
+  <si>
+    <t>CA-66Q40L5H</t>
+  </si>
+  <si>
+    <t>CA-FVCPV7Z6</t>
+  </si>
+  <si>
+    <t>CA-94RV63V0</t>
+  </si>
+  <si>
+    <t>CA-F1DFS69H</t>
+  </si>
+  <si>
+    <t>CA-7S0WFUST</t>
+  </si>
+  <si>
+    <t>CA-ASYY2BPD</t>
+  </si>
+  <si>
+    <t>CA-VZM6NS56</t>
+  </si>
+  <si>
+    <t>CA-QLRKYYO0</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1149,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>

</xml_diff>